<commit_message>
Run on noiseless signal with changed network
</commit_message>
<xml_diff>
--- a/Results/New/Plots/Plot.xlsx
+++ b/Results/New/Plots/Plot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAA_Projecten\LSTM_Periodic_Function\Results\New\Plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A481E1-74C5-490F-8E0F-3554DB4BD9E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A4973D-660D-47B4-904E-430636FAA2EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,7 +182,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>([4]Outliers_P_1percent!$B$3,[4]Outliers_P_1percent!$B$5,[4]Outliers_P_1percent!$B$7,[4]Outliers_P_1percent!$B$9,[4]Outliers_P_1percent!$B$11,[4]Outliers_P_1percent!$B$13)</c:f>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -209,7 +209,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>([1]Noiseless!$C$3,[1]Noiseless!$C$5,[1]Noiseless!$C$7,[1]Noiseless!$C$9,[1]Noiseless!$C$11,[1]Noiseless!$C$13)</c:f>
+              <c:f>([2]Noiseless!$C$3,[2]Noiseless!$C$5,[2]Noiseless!$C$7,[2]Noiseless!$C$9,[2]Noiseless!$C$11,[2]Noiseless!$C$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -242,15 +242,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
-            <c:v>Gaussian (dev=2)</c:v>
+            <c:v>Noiseless + stdv</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -261,7 +261,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>([4]Outliers_P_1percent!$B$3,[4]Outliers_P_1percent!$B$5,[4]Outliers_P_1percent!$B$7,[4]Outliers_P_1percent!$B$9,[4]Outliers_P_1percent!$B$11,[4]Outliers_P_1percent!$B$13)</c:f>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -284,39 +284,41 @@
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>([2]Gaussian_dev_2!$C$3,[2]Gaussian_dev_2!$C$5,[2]Gaussian_dev_2!$C$7,[2]Gaussian_dev_2!$C$9,[2]Gaussian_dev_2!$C$11,[2]Gaussian_dev_2!$C$13)</c:f>
+              <c:f>([2]Noiseless!$E$3,[2]Noiseless!$E$5,[2]Noiseless!$E$7,[2]Noiseless!$E$9,[2]Noiseless!$E$11,[2]Noiseless!$E$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.53851910000000003</c:v>
+                  <c:v>0.20768525800000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64606786000000005</c:v>
+                  <c:v>0.12508976599999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66135909999999998</c:v>
+                  <c:v>9.1817866999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60077590000000003</c:v>
+                  <c:v>0.19488364</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15163157999999999</c:v>
+                  <c:v>0.21993918000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9967646999999997E-2</c:v>
+                  <c:v>4.2730878999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-09E8-462E-A479-82A3EAE6E86B}"/>
+              <c16:uniqueId val="{00000002-09E8-462E-A479-82A3EAE6E86B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -340,7 +342,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>([4]Outliers_P_1percent!$B$3,[4]Outliers_P_1percent!$B$5,[4]Outliers_P_1percent!$B$7,[4]Outliers_P_1percent!$B$9,[4]Outliers_P_1percent!$B$11,[4]Outliers_P_1percent!$B$13)</c:f>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -367,7 +369,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('[3]Outliers_P_0,01percent'!$C$3,'[3]Outliers_P_0,01percent'!$C$5,'[3]Outliers_P_0,01percent'!$C$7,'[3]Outliers_P_0,01percent'!$C$9,'[3]Outliers_P_0,01percent'!$C$11,'[3]Outliers_P_0,01percent'!$C$13)</c:f>
+              <c:f>('[4]Outliers_P_0,01percent'!$C$3,'[4]Outliers_P_0,01percent'!$C$5,'[4]Outliers_P_0,01percent'!$C$7,'[4]Outliers_P_0,01percent'!$C$9,'[4]Outliers_P_0,01percent'!$C$11,'[4]Outliers_P_0,01percent'!$C$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -403,7 +405,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>Outliers (P=0.0001) stdv</c:v>
+            <c:v>Outliers (P=0.0001) + stdv</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -419,7 +421,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>([4]Outliers_P_1percent!$B$3,[4]Outliers_P_1percent!$B$5,[4]Outliers_P_1percent!$B$7,[4]Outliers_P_1percent!$B$9,[4]Outliers_P_1percent!$B$11,[4]Outliers_P_1percent!$B$13)</c:f>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -446,7 +448,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('[3]Outliers_P_0,01percent'!$E$3,'[3]Outliers_P_0,01percent'!$E$5,'[3]Outliers_P_0,01percent'!$E$7,'[3]Outliers_P_0,01percent'!$E$9,'[3]Outliers_P_0,01percent'!$E$11,'[3]Outliers_P_0,01percent'!$E$13)</c:f>
+              <c:f>('[4]Outliers_P_0,01percent'!$E$3,'[4]Outliers_P_0,01percent'!$E$5,'[4]Outliers_P_0,01percent'!$E$7,'[4]Outliers_P_0,01percent'!$E$9,'[4]Outliers_P_0,01percent'!$E$11,'[4]Outliers_P_0,01percent'!$E$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -454,13 +456,13 @@
                   <c:v>0.25914482999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7345936000000005E-2</c:v>
+                  <c:v>4.7345935999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.4472772999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18660686399999998</c:v>
+                  <c:v>0.18660686400000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.61843934</c:v>
@@ -500,7 +502,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>([4]Outliers_P_1percent!$B$3,[4]Outliers_P_1percent!$B$5,[4]Outliers_P_1percent!$B$7,[4]Outliers_P_1percent!$B$9,[4]Outliers_P_1percent!$B$11,[4]Outliers_P_1percent!$B$13)</c:f>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -527,7 +529,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>([4]Outliers_P_1percent!$C$3,[4]Outliers_P_1percent!$C$5,[4]Outliers_P_1percent!$C$7,[4]Outliers_P_1percent!$C$9,[4]Outliers_P_1percent!$C$11,[4]Outliers_P_1percent!$C$13)</c:f>
+              <c:f>([1]Outliers_P_1percent!$C$3,[1]Outliers_P_1percent!$C$5,[1]Outliers_P_1percent!$C$7,[1]Outliers_P_1percent!$C$9,[1]Outliers_P_1percent!$C$11,[1]Outliers_P_1percent!$C$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -563,7 +565,7 @@
           <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>Outliers (P=0.01) stdv</c:v>
+            <c:v>Outliers (P=0.01) + stdv</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -581,7 +583,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>([4]Outliers_P_1percent!$B$3,[4]Outliers_P_1percent!$B$5,[4]Outliers_P_1percent!$B$7,[4]Outliers_P_1percent!$B$9,[4]Outliers_P_1percent!$B$11,[4]Outliers_P_1percent!$B$13)</c:f>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -608,7 +610,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>([4]Outliers_P_1percent!$E$3,[4]Outliers_P_1percent!$E$5,[4]Outliers_P_1percent!$E$7,[4]Outliers_P_1percent!$E$9,[4]Outliers_P_1percent!$E$11,[4]Outliers_P_1percent!$E$13)</c:f>
+              <c:f>([1]Outliers_P_1percent!$E$3,[1]Outliers_P_1percent!$E$5,[1]Outliers_P_1percent!$E$7,[1]Outliers_P_1percent!$E$9,[1]Outliers_P_1percent!$E$11,[1]Outliers_P_1percent!$E$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -616,7 +618,7 @@
                   <c:v>9.0977986999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6007583000000005E-2</c:v>
+                  <c:v>4.6007582999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.7946035999999999E-2</c:v>
@@ -625,7 +627,7 @@
                   <c:v>9.0689188000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23434808099999999</c:v>
+                  <c:v>0.23434808100000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.107658305</c:v>
@@ -698,7 +700,7 @@
           <c:idx val="9"/>
           <c:order val="9"/>
           <c:tx>
-            <c:v>Disturbing (A=4, F=2) stdv</c:v>
+            <c:v>Disturbing (A=4, F=2) + stdv</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -763,15 +765,15 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:idx val="2"/>
+                <c:order val="2"/>
                 <c:tx>
-                  <c:v>Noiseless stdv</c:v>
+                  <c:v>Gaussian (dev=2)</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent3"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -785,7 +787,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>([4]Outliers_P_1percent!$B$3,[4]Outliers_P_1percent!$B$5,[4]Outliers_P_1percent!$B$7,[4]Outliers_P_1percent!$B$9,[4]Outliers_P_1percent!$B$11,[4]Outliers_P_1percent!$B$13)</c15:sqref>
+                          <c15:sqref>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -818,7 +820,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>([1]Noiseless!$E$3,[1]Noiseless!$E$5,[1]Noiseless!$E$7,[1]Noiseless!$E$9,[1]Noiseless!$E$11,[1]Noiseless!$E$13)</c15:sqref>
+                          <c15:sqref>([3]Gaussian_dev_2!$C$3,[3]Gaussian_dev_2!$C$5,[3]Gaussian_dev_2!$C$7,[3]Gaussian_dev_2!$C$9,[3]Gaussian_dev_2!$C$11,[3]Gaussian_dev_2!$C$13)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -826,22 +828,22 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>0.20768525800000001</c:v>
+                        <c:v>0.53851910000000003</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.12508976599999999</c:v>
+                        <c:v>0.64606786000000005</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>9.1817866999999997E-2</c:v>
+                        <c:v>0.66135909999999998</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.19488364</c:v>
+                        <c:v>0.60077590000000003</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0.21993918000000001</c:v>
+                        <c:v>0.15163157999999999</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>4.2730878999999999E-2</c:v>
+                        <c:v>4.9967646999999997E-2</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -849,7 +851,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-09E8-462E-A479-82A3EAE6E86B}"/>
+                    <c16:uniqueId val="{00000003-09E8-462E-A479-82A3EAE6E86B}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -859,7 +861,7 @@
                 <c:idx val="3"/>
                 <c:order val="3"/>
                 <c:tx>
-                  <c:v>Gaussian (dev=2) stdv</c:v>
+                  <c:v>Gaussian (dev=2) + stdv</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
@@ -875,10 +877,10 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>([4]Outliers_P_1percent!$B$3,[4]Outliers_P_1percent!$B$5,[4]Outliers_P_1percent!$B$7,[4]Outliers_P_1percent!$B$9,[4]Outliers_P_1percent!$B$11,[4]Outliers_P_1percent!$B$13)</c15:sqref>
+                          <c15:sqref>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -908,10 +910,10 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>([2]Gaussian_dev_2!$E$3,[2]Gaussian_dev_2!$E$5,[2]Gaussian_dev_2!$E$7,[2]Gaussian_dev_2!$E$9,[2]Gaussian_dev_2!$E$11,[2]Gaussian_dev_2!$E$13)</c15:sqref>
+                          <c15:sqref>([3]Gaussian_dev_2!$E$3,[3]Gaussian_dev_2!$E$5,[3]Gaussian_dev_2!$E$7,[3]Gaussian_dev_2!$E$9,[3]Gaussian_dev_2!$E$11,[3]Gaussian_dev_2!$E$13)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -919,22 +921,1089 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>0.57346265000000007</c:v>
+                        <c:v>0.57346264999999996</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.83166586000000009</c:v>
+                        <c:v>0.83166585999999998</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.79034615999999991</c:v>
+                        <c:v>0.79034616000000002</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.86805240000000006</c:v>
+                        <c:v>0.86805239999999995</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0.22163942999999997</c:v>
+                        <c:v>0.22163943</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>7.148252699999999E-2</c:v>
+                        <c:v>7.1482527000000004E-2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-09E8-462E-A479-82A3EAE6E86B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="568129192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>k</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="568121648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="568121648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean Absolute Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="568129192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sampling interval 1 minute</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Noiseless</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>([2]Noiseless!$C$27,[2]Noiseless!$C$29,[2]Noiseless!$C$31,[2]Noiseless!$C$33,[2]Noiseless!$C$35,[2]Noiseless!$C$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.9281062999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7827525</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9206047000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1230729999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7202489999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.2012176999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C373-4CA7-94BB-F6F8A779EDF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Noiseless + stdv</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>([2]Noiseless!$E$27,[2]Noiseless!$E$29,[2]Noiseless!$E$31,[2]Noiseless!$E$33,[2]Noiseless!$E$35,[2]Noiseless!$E$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.1581752999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8635163000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.9055532999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6264216000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0200089999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7753344000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-C373-4CA7-94BB-F6F8A779EDF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Outliers (P=0.0001)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('[4]Outliers_P_0,01percent'!$C$27,'[4]Outliers_P_0,01percent'!$C$29,'[4]Outliers_P_0,01percent'!$C$31,'[4]Outliers_P_0,01percent'!$C$33,'[4]Outliers_P_0,01percent'!$C$35,'[4]Outliers_P_0,01percent'!$C$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.9174980000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7736793000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0494859999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2639545999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5728790000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.1499867000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C373-4CA7-94BB-F6F8A779EDF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Outliers (P=0.0001) + stdv</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('[4]Outliers_P_0,01percent'!$E$27,'[4]Outliers_P_0,01percent'!$E$29,'[4]Outliers_P_0,01percent'!$E$31,'[4]Outliers_P_0,01percent'!$E$33,'[4]Outliers_P_0,01percent'!$E$35,'[4]Outliers_P_0,01percent'!$E$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.9042486000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8421853000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0632757</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3859697999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2894006999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.2052104000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C373-4CA7-94BB-F6F8A779EDF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Outliers (P=0.01)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>([1]Outliers_P_1percent!$C$27,[1]Outliers_P_1percent!$C$29,[1]Outliers_P_1percent!$C$31,[1]Outliers_P_1percent!$C$33,[1]Outliers_P_1percent!$C$35,[1]Outliers_P_1percent!$C$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.6744729999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6466450000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9847999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2733355</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9323750000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9651145999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C373-4CA7-94BB-F6F8A779EDF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Outliers (P=0.01) + stdv</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>([1]Outliers_P_1percent!$E$27,[1]Outliers_P_1percent!$E$29,[1]Outliers_P_1percent!$E$31,[1]Outliers_P_1percent!$E$33,[1]Outliers_P_1percent!$E$35,[1]Outliers_P_1percent!$E$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.7805914000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8017806000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0919098</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.4146327999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8123197999999991</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7177038000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C373-4CA7-94BB-F6F8A779EDF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Disturbing (A=4, F=2)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>([5]Disturbing_A_4_F_2!$C$27,[5]Disturbing_A_4_F_2!$C$29,[5]Disturbing_A_4_F_2!$C$31,[5]Disturbing_A_4_F_2!$C$33,[5]Disturbing_A_4_F_2!$C$35,[5]Disturbing_A_4_F_2!$C$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.9281205999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0001984000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8297204999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0018599999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8554396999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.7963256999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C373-4CA7-94BB-F6F8A779EDF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Disturbing (A=4, F=2) + stdv</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>([5]Disturbing_A_4_F_2!$E$27,[5]Disturbing_A_4_F_2!$E$29,[5]Disturbing_A_4_F_2!$E$31,[5]Disturbing_A_4_F_2!$E$33,[5]Disturbing_A_4_F_2!$E$35,[5]Disturbing_A_4_F_2!$E$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.1582106000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.059606799999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0660644000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2847086000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.3125839999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5374391000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-C373-4CA7-94BB-F6F8A779EDF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="568129192"/>
+        <c:axId val="568121648"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>Gaussian (dev=2)</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>32</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>([3]Gaussian_dev_2!$C$27,[3]Gaussian_dev_2!$C$29,[3]Gaussian_dev_2!$C$31,[3]Gaussian_dev_2!$C$33,[3]Gaussian_dev_2!$C$35,[3]Gaussian_dev_2!$C$37)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>5.9231943999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>6.8823543000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5.6261653999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5.8334599999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>6.1890016000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6.9570230000000004</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -942,7 +2011,100 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000004-09E8-462E-A479-82A3EAE6E86B}"/>
+                    <c16:uniqueId val="{00000001-C373-4CA7-94BB-F6F8A779EDF3}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>Gaussian (dev=2) + stdv</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>([1]Outliers_P_1percent!$B$3,[1]Outliers_P_1percent!$B$5,[1]Outliers_P_1percent!$B$7,[1]Outliers_P_1percent!$B$9,[1]Outliers_P_1percent!$B$11,[1]Outliers_P_1percent!$B$13)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>32</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>([3]Gaussian_dev_2!$E$27,[3]Gaussian_dev_2!$E$29,[3]Gaussian_dev_2!$E$31,[3]Gaussian_dev_2!$E$33,[3]Gaussian_dev_2!$E$35,[3]Gaussian_dev_2!$E$37)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>9.1462866999999992</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>9.8566947000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>8.4815281000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>9.5362176000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>9.6164848999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>9.9765937999999998</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000009-C373-4CA7-94BB-F6F8A779EDF3}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1286,7 +2448,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1840,6 +3558,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AED0758-67AD-4B30-ABDB-0B6B2610460E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1847,7 +3603,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Noiseless"/>
+      <sheetName val="Outliers_P_1percent"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -1856,13 +3612,10 @@
             <v>1</v>
           </cell>
           <cell r="C3">
-            <v>0.16853835</v>
-          </cell>
-          <cell r="D3">
-            <v>3.9146908000000001E-2</v>
+            <v>5.5789859999999997E-2</v>
           </cell>
           <cell r="E3">
-            <v>0.20768525800000001</v>
+            <v>9.0977986999999996E-2</v>
           </cell>
         </row>
         <row r="5">
@@ -1870,13 +3623,10 @@
             <v>2</v>
           </cell>
           <cell r="C5">
-            <v>8.3168809999999996E-2</v>
-          </cell>
-          <cell r="D5">
-            <v>4.1920956000000002E-2</v>
+            <v>3.4952490000000003E-2</v>
           </cell>
           <cell r="E5">
-            <v>0.12508976599999999</v>
+            <v>4.6007582999999998E-2</v>
           </cell>
         </row>
         <row r="7">
@@ -1884,13 +3634,10 @@
             <v>4</v>
           </cell>
           <cell r="C7">
-            <v>5.6844205000000002E-2</v>
-          </cell>
-          <cell r="D7">
-            <v>3.4973662000000003E-2</v>
+            <v>3.5214599999999999E-2</v>
           </cell>
           <cell r="E7">
-            <v>9.1817866999999997E-2</v>
+            <v>5.7946035999999999E-2</v>
           </cell>
         </row>
         <row r="9">
@@ -1898,13 +3645,10 @@
             <v>8</v>
           </cell>
           <cell r="C9">
-            <v>0.11466704</v>
-          </cell>
-          <cell r="D9">
-            <v>8.0216599999999999E-2</v>
+            <v>5.9908148000000001E-2</v>
           </cell>
           <cell r="E9">
-            <v>0.19488364</v>
+            <v>9.0689188000000004E-2</v>
           </cell>
         </row>
         <row r="11">
@@ -1912,13 +3656,10 @@
             <v>16</v>
           </cell>
           <cell r="C11">
-            <v>0.11709881599999999</v>
-          </cell>
-          <cell r="D11">
-            <v>0.102840364</v>
+            <v>0.119210966</v>
           </cell>
           <cell r="E11">
-            <v>0.21993918000000001</v>
+            <v>0.23434808100000001</v>
           </cell>
         </row>
         <row r="13">
@@ -1926,13 +3667,58 @@
             <v>32</v>
           </cell>
           <cell r="C13">
-            <v>2.4005054000000001E-2</v>
-          </cell>
-          <cell r="D13">
-            <v>1.8725825000000001E-2</v>
+            <v>5.8926544999999997E-2</v>
           </cell>
           <cell r="E13">
-            <v>4.2730878999999999E-2</v>
+            <v>0.107658305</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>6.6744729999999999</v>
+          </cell>
+          <cell r="E27">
+            <v>9.7805914000000005</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>6.6466450000000004</v>
+          </cell>
+          <cell r="E29">
+            <v>9.8017806000000007</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>6.9847999999999999</v>
+          </cell>
+          <cell r="E31">
+            <v>10.0919098</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>6.2733355</v>
+          </cell>
+          <cell r="E33">
+            <v>9.4146327999999997</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>6.9323750000000004</v>
+          </cell>
+          <cell r="E35">
+            <v>9.8123197999999991</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>5.9651145999999997</v>
+          </cell>
+          <cell r="E37">
+            <v>8.7177038000000007</v>
           </cell>
         </row>
       </sheetData>
@@ -1945,74 +3731,104 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Gaussian_dev_2"/>
+      <sheetName val="Noiseless"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="B3">
-            <v>1</v>
-          </cell>
           <cell r="C3">
-            <v>0.53851910000000003</v>
+            <v>0.16853835</v>
           </cell>
           <cell r="E3">
-            <v>0.57346265000000007</v>
+            <v>0.20768525800000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="B5">
-            <v>2</v>
-          </cell>
           <cell r="C5">
-            <v>0.64606786000000005</v>
+            <v>8.3168809999999996E-2</v>
           </cell>
           <cell r="E5">
-            <v>0.83166586000000009</v>
+            <v>0.12508976599999999</v>
           </cell>
         </row>
         <row r="7">
-          <cell r="B7">
-            <v>4</v>
-          </cell>
           <cell r="C7">
-            <v>0.66135909999999998</v>
+            <v>5.6844205000000002E-2</v>
           </cell>
           <cell r="E7">
-            <v>0.79034615999999991</v>
+            <v>9.1817866999999997E-2</v>
           </cell>
         </row>
         <row r="9">
-          <cell r="B9">
-            <v>8</v>
-          </cell>
           <cell r="C9">
-            <v>0.60077590000000003</v>
+            <v>0.11466704</v>
           </cell>
           <cell r="E9">
-            <v>0.86805240000000006</v>
+            <v>0.19488364</v>
           </cell>
         </row>
         <row r="11">
-          <cell r="B11">
-            <v>16</v>
-          </cell>
           <cell r="C11">
-            <v>0.15163157999999999</v>
+            <v>0.11709881599999999</v>
           </cell>
           <cell r="E11">
-            <v>0.22163942999999997</v>
+            <v>0.21993918000000001</v>
           </cell>
         </row>
         <row r="13">
-          <cell r="B13">
-            <v>32</v>
-          </cell>
           <cell r="C13">
-            <v>4.9967646999999997E-2</v>
+            <v>2.4005054000000001E-2</v>
           </cell>
           <cell r="E13">
-            <v>7.148252699999999E-2</v>
+            <v>4.2730878999999999E-2</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>5.9281062999999996</v>
+          </cell>
+          <cell r="E27">
+            <v>9.1581752999999999</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>6.7827525</v>
+          </cell>
+          <cell r="E29">
+            <v>9.8635163000000006</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>5.9206047000000002</v>
+          </cell>
+          <cell r="E31">
+            <v>8.9055532999999993</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>6.1230729999999998</v>
+          </cell>
+          <cell r="E33">
+            <v>9.6264216000000005</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>5.7202489999999999</v>
+          </cell>
+          <cell r="E35">
+            <v>9.0200089999999999</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>6.2012176999999999</v>
+          </cell>
+          <cell r="E37">
+            <v>8.7753344000000002</v>
           </cell>
         </row>
       </sheetData>
@@ -2025,56 +3841,104 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Outliers_P_0,01percent"/>
+      <sheetName val="Gaussian_dev_2"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
           <cell r="C3">
-            <v>0.15743892000000001</v>
+            <v>0.53851910000000003</v>
           </cell>
           <cell r="E3">
-            <v>0.25914482999999999</v>
+            <v>0.57346264999999996</v>
           </cell>
         </row>
         <row r="5">
           <cell r="C5">
-            <v>3.2197410000000003E-2</v>
+            <v>0.64606786000000005</v>
           </cell>
           <cell r="E5">
-            <v>4.7345936000000005E-2</v>
+            <v>0.83166585999999998</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>2.0049522E-2</v>
+            <v>0.66135909999999998</v>
           </cell>
           <cell r="E7">
-            <v>3.4472772999999998E-2</v>
+            <v>0.79034616000000002</v>
           </cell>
         </row>
         <row r="9">
           <cell r="C9">
-            <v>8.5128783999999999E-2</v>
+            <v>0.60077590000000003</v>
           </cell>
           <cell r="E9">
-            <v>0.18660686399999998</v>
+            <v>0.86805239999999995</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>0.32770769999999999</v>
+            <v>0.15163157999999999</v>
           </cell>
           <cell r="E11">
-            <v>0.61843934</v>
+            <v>0.22163943</v>
           </cell>
         </row>
         <row r="13">
           <cell r="C13">
-            <v>0.106302574</v>
+            <v>4.9967646999999997E-2</v>
           </cell>
           <cell r="E13">
-            <v>0.19791658400000001</v>
+            <v>7.1482527000000004E-2</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>5.9231943999999999</v>
+          </cell>
+          <cell r="E27">
+            <v>9.1462866999999992</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>6.8823543000000003</v>
+          </cell>
+          <cell r="E29">
+            <v>9.8566947000000003</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>5.6261653999999997</v>
+          </cell>
+          <cell r="E31">
+            <v>8.4815281000000002</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>5.8334599999999996</v>
+          </cell>
+          <cell r="E33">
+            <v>9.5362176000000005</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>6.1890016000000001</v>
+          </cell>
+          <cell r="E35">
+            <v>9.6164848999999997</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>6.9570230000000004</v>
+          </cell>
+          <cell r="E37">
+            <v>9.9765937999999998</v>
           </cell>
         </row>
       </sheetData>
@@ -2087,74 +3951,104 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Outliers_P_1percent"/>
+      <sheetName val="Outliers_P_0,01percent"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="B3">
-            <v>1</v>
-          </cell>
           <cell r="C3">
-            <v>5.5789859999999997E-2</v>
+            <v>0.15743892000000001</v>
           </cell>
           <cell r="E3">
-            <v>9.0977986999999996E-2</v>
+            <v>0.25914482999999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="B5">
-            <v>2</v>
-          </cell>
           <cell r="C5">
-            <v>3.4952490000000003E-2</v>
+            <v>3.2197410000000003E-2</v>
           </cell>
           <cell r="E5">
-            <v>4.6007583000000005E-2</v>
+            <v>4.7345935999999998E-2</v>
           </cell>
         </row>
         <row r="7">
-          <cell r="B7">
-            <v>4</v>
-          </cell>
           <cell r="C7">
-            <v>3.5214599999999999E-2</v>
+            <v>2.0049522E-2</v>
           </cell>
           <cell r="E7">
-            <v>5.7946035999999999E-2</v>
+            <v>3.4472772999999998E-2</v>
           </cell>
         </row>
         <row r="9">
-          <cell r="B9">
-            <v>8</v>
-          </cell>
           <cell r="C9">
-            <v>5.9908148000000001E-2</v>
+            <v>8.5128783999999999E-2</v>
           </cell>
           <cell r="E9">
-            <v>9.0689188000000004E-2</v>
+            <v>0.18660686400000001</v>
           </cell>
         </row>
         <row r="11">
-          <cell r="B11">
-            <v>16</v>
-          </cell>
           <cell r="C11">
-            <v>0.119210966</v>
+            <v>0.32770769999999999</v>
           </cell>
           <cell r="E11">
-            <v>0.23434808099999999</v>
+            <v>0.61843934</v>
           </cell>
         </row>
         <row r="13">
-          <cell r="B13">
-            <v>32</v>
-          </cell>
           <cell r="C13">
-            <v>5.8926544999999997E-2</v>
+            <v>0.106302574</v>
           </cell>
           <cell r="E13">
-            <v>0.107658305</v>
+            <v>0.19791658400000001</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>6.9174980000000001</v>
+          </cell>
+          <cell r="E27">
+            <v>9.9042486000000007</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>6.7736793000000004</v>
+          </cell>
+          <cell r="E29">
+            <v>9.8421853000000006</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>7.0494859999999999</v>
+          </cell>
+          <cell r="E31">
+            <v>10.0632757</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>6.2639545999999999</v>
+          </cell>
+          <cell r="E33">
+            <v>9.3859697999999998</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>6.5728790000000004</v>
+          </cell>
+          <cell r="E35">
+            <v>9.2894006999999998</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>6.1499867000000004</v>
+          </cell>
+          <cell r="E37">
+            <v>9.2052104000000003</v>
           </cell>
         </row>
       </sheetData>
@@ -2217,6 +4111,54 @@
           </cell>
           <cell r="E13">
             <v>1.1537040199999999</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>5.9281205999999997</v>
+          </cell>
+          <cell r="E27">
+            <v>9.1582106000000003</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>7.0001984000000004</v>
+          </cell>
+          <cell r="E29">
+            <v>10.059606799999999</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>5.8297204999999996</v>
+          </cell>
+          <cell r="E31">
+            <v>9.0660644000000001</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>6.0018599999999998</v>
+          </cell>
+          <cell r="E33">
+            <v>9.2847086000000001</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>5.8554396999999998</v>
+          </cell>
+          <cell r="E35">
+            <v>9.3125839999999993</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>6.7963256999999997</v>
+          </cell>
+          <cell r="E37">
+            <v>9.5374391000000003</v>
           </cell>
         </row>
       </sheetData>
@@ -2490,7 +4432,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>